<commit_message>
terms added in exclude list
</commit_message>
<xml_diff>
--- a/data/exclude_list.xlsx
+++ b/data/exclude_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ICTO-EB\Google Drive\myThesis\evaluation_testdataSet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ICTO-EB\github_project\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15138F49-3B4A-424C-A53F-60E78059C6CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD130E52-6741-4594-B762-4BBBDD2CBCD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{900FE936-8A05-4F79-B436-47D13D5562F9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="647">
   <si>
     <t>above-mentioned</t>
   </si>
@@ -1965,6 +1965,15 @@
   </si>
   <si>
     <t>gements</t>
+  </si>
+  <si>
+    <t>diversoups</t>
+  </si>
+  <si>
+    <t>longitudinal</t>
+  </si>
+  <si>
+    <t>three-wave</t>
   </si>
 </sst>
 </file>
@@ -2363,10 +2372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277838AB-5E92-4D92-9401-2048F1AC9206}">
-  <dimension ref="A1:A644"/>
+  <dimension ref="A1:A647"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A632" workbookViewId="0">
-      <selection activeCell="A643" sqref="A643"/>
+    <sheetView tabSelected="1" topLeftCell="A623" workbookViewId="0">
+      <selection activeCell="H634" sqref="H634"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5594,6 +5603,21 @@
         <v>643</v>
       </c>
     </row>
+    <row r="645" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A645" s="3" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="646" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A646" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="647" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A647" t="s">
+        <v>646</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>